<commit_message>
Gradient Descent Learning (SISO)
</commit_message>
<xml_diff>
--- a/Basic Deep Learning/Gradient Descent.xlsx
+++ b/Basic Deep Learning/Gradient Descent.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\learning\Grokking-DL\Basic Deep Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\30__Sandbox_Learning\Grokking-DL\Basic Deep Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40816503-B8D0-43FF-BED3-B40CAE37A9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D5C485-BB1D-4973-8B5A-7FE903486FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
   <si>
     <t>SISO - Single Input Single Output</t>
   </si>
@@ -1099,10 +1099,6 @@
       </rPr>
       <t>11</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">STILL HAS ERROR &amp; 
-NEED LEARNING? </t>
   </si>
   <si>
     <t>Error != 0</t>
@@ -2355,9 +2351,6 @@
     <t>Total Error</t>
   </si>
   <si>
-    <t>CONTINUE LEARNING ?</t>
-  </si>
-  <si>
     <t>Continue ?</t>
   </si>
   <si>
@@ -2422,6 +2415,9 @@
       </rPr>
       <t>3</t>
     </r>
+  </si>
+  <si>
+    <t>NEED LEARNING ?</t>
   </si>
 </sst>
 </file>
@@ -2762,41 +2758,44 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2815,9 +2814,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5418,8 +5414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6:R7"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32:R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5444,13 +5440,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -5524,38 +5520,38 @@
       <c r="R5" s="9"/>
     </row>
     <row r="6" spans="2:22" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="25"/>
-      <c r="F6" s="21"/>
-      <c r="H6" s="18" t="s">
+      <c r="F6" s="26"/>
+      <c r="H6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="K6" s="20" t="s">
+      <c r="I6" s="23"/>
+      <c r="K6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="21"/>
-      <c r="N6" s="18" t="s">
+      <c r="L6" s="26"/>
+      <c r="N6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="R6" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="U6" s="18" t="s">
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="R6" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="U6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="V6" s="18"/>
+      <c r="V6" s="23"/>
     </row>
     <row r="7" spans="2:22" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="6"/>
       <c r="D7" s="13" t="s">
         <v>5</v>
@@ -5587,18 +5583,18 @@
       <c r="P7" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="R7" s="23"/>
-      <c r="U7" s="16" t="str">
+      <c r="R7" s="20"/>
+      <c r="U7" s="19" t="str">
         <f>H7</f>
         <v>Weight</v>
       </c>
-      <c r="V7" s="16" t="str">
+      <c r="V7" s="19" t="str">
         <f>L7</f>
         <v>Error</v>
       </c>
     </row>
     <row r="8" spans="2:22" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="6"/>
       <c r="D8" s="14" t="s">
         <v>31</v>
@@ -5635,12 +5631,12 @@
       </c>
       <c r="Q8" s="15"/>
       <c r="R8" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
     </row>
     <row r="9" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
@@ -5659,23 +5655,23 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f>F9*H9</f>
+        <f t="shared" ref="I9:I28" si="0">F9*H9</f>
         <v>0</v>
       </c>
       <c r="K9" s="2">
-        <f>I9-D9</f>
+        <f t="shared" ref="K9:K28" si="1">I9-D9</f>
         <v>-8</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" ref="L9:L28" si="0">ROUND(POWER(K9,2), 5)</f>
+        <f t="shared" ref="L9:L28" si="2">ROUND(POWER(K9,2), 5)</f>
         <v>64</v>
       </c>
       <c r="N9" s="2">
-        <f>2*F9*K9</f>
+        <f t="shared" ref="N9:N28" si="3">2*F9*K9</f>
         <v>-1.6</v>
       </c>
       <c r="O9" s="2">
-        <f>E9*N9</f>
+        <f t="shared" ref="O9:O28" si="4">E9*N9</f>
         <v>-28.8</v>
       </c>
       <c r="P9" s="2">
@@ -5717,23 +5713,23 @@
         <v>28.8</v>
       </c>
       <c r="I10" s="2">
-        <f>F10*H10</f>
+        <f t="shared" si="0"/>
         <v>2.8800000000000003</v>
       </c>
       <c r="K10" s="2">
-        <f>I10-D10</f>
+        <f t="shared" si="1"/>
         <v>-5.1199999999999992</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>26.214400000000001</v>
       </c>
       <c r="N10" s="2">
-        <f>2*F10*K10</f>
+        <f t="shared" si="3"/>
         <v>-1.0239999999999998</v>
       </c>
       <c r="O10" s="2">
-        <f>E10*N10</f>
+        <f t="shared" si="4"/>
         <v>-18.431999999999995</v>
       </c>
       <c r="P10" s="2">
@@ -5741,1059 +5737,1059 @@
         <v>47.231999999999999</v>
       </c>
       <c r="R10" s="7" t="b">
-        <f t="shared" ref="R10:R28" si="1">(L10&lt;&gt;0)</f>
+        <f t="shared" ref="R10:R28" si="5">(L10&lt;&gt;0)</f>
         <v>1</v>
       </c>
       <c r="U10" s="2">
-        <f t="shared" ref="U10:U25" si="2">H10</f>
+        <f t="shared" ref="U10:U25" si="6">H10</f>
         <v>28.8</v>
       </c>
       <c r="V10" s="2">
-        <f t="shared" ref="V10:V25" si="3">L10</f>
+        <f t="shared" ref="V10:V25" si="7">L10</f>
         <v>26.214400000000001</v>
       </c>
     </row>
     <row r="11" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
-        <f t="shared" ref="B11:B22" si="4">B10+1</f>
+        <f t="shared" ref="B11:B22" si="8">B10+1</f>
         <v>3</v>
       </c>
       <c r="D11" s="7">
-        <f t="shared" ref="D11:D22" si="5">D10</f>
+        <f t="shared" ref="D11:D22" si="9">D10</f>
         <v>8</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" ref="E11:E22" si="6">E10</f>
+        <f t="shared" ref="E11:E22" si="10">E10</f>
         <v>18</v>
       </c>
       <c r="F11" s="7">
-        <f>F10</f>
+        <f t="shared" ref="F11:F28" si="11">F10</f>
         <v>0.1</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" ref="H11:H22" si="7">P10</f>
+        <f t="shared" ref="H11:H22" si="12">P10</f>
         <v>47.231999999999999</v>
       </c>
       <c r="I11" s="2">
-        <f>F11*H11</f>
+        <f t="shared" si="0"/>
         <v>4.7232000000000003</v>
       </c>
       <c r="K11" s="2">
-        <f>I11-D11</f>
+        <f t="shared" si="1"/>
         <v>-3.2767999999999997</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.73742</v>
       </c>
       <c r="N11" s="2">
-        <f>2*F11*K11</f>
+        <f t="shared" si="3"/>
         <v>-0.65535999999999994</v>
       </c>
       <c r="O11" s="2">
-        <f>E11*N11</f>
+        <f t="shared" si="4"/>
         <v>-11.796479999999999</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" ref="P11:P22" si="8">H11-O11</f>
+        <f t="shared" ref="P11:P22" si="13">H11-O11</f>
         <v>59.028480000000002</v>
       </c>
       <c r="R11" s="7" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>47.231999999999999</v>
       </c>
       <c r="V11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>10.73742</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="12"/>
+        <v>59.028480000000002</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>5.9028480000000005</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.0971519999999995</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="2"/>
+        <v>4.3980499999999996</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.41943039999999993</v>
+      </c>
+      <c r="O12" s="2">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="D12" s="7">
+        <v>-7.5497471999999988</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="13"/>
+        <v>66.578227200000001</v>
+      </c>
+      <c r="R12" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="U12" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F12" s="7">
-        <f>F11</f>
-        <v>0.1</v>
-      </c>
-      <c r="H12" s="2">
+        <v>59.028480000000002</v>
+      </c>
+      <c r="V12" s="2">
         <f t="shared" si="7"/>
-        <v>59.028480000000002</v>
-      </c>
-      <c r="I12" s="2">
-        <f>F12*H12</f>
-        <v>5.9028480000000005</v>
-      </c>
-      <c r="K12" s="2">
-        <f>I12-D12</f>
-        <v>-2.0971519999999995</v>
-      </c>
-      <c r="L12" s="2">
-        <f t="shared" si="0"/>
-        <v>4.3980499999999996</v>
-      </c>
-      <c r="N12" s="2">
-        <f>2*F12*K12</f>
-        <v>-0.41943039999999993</v>
-      </c>
-      <c r="O12" s="2">
-        <f>E12*N12</f>
-        <v>-7.5497471999999988</v>
-      </c>
-      <c r="P12" s="2">
-        <f t="shared" si="8"/>
-        <v>66.578227200000001</v>
-      </c>
-      <c r="R12" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U12" s="2">
-        <f t="shared" si="2"/>
-        <v>59.028480000000002</v>
-      </c>
-      <c r="V12" s="2">
-        <f t="shared" si="3"/>
         <v>4.3980499999999996</v>
       </c>
     </row>
     <row r="13" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="12"/>
+        <v>66.578227200000001</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>6.6578227200000004</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.3421772799999996</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8014399999999999</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.26843545599999991</v>
+      </c>
+      <c r="O13" s="2">
         <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="D13" s="7">
+        <v>-4.831838207999998</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="13"/>
+        <v>71.410065407999994</v>
+      </c>
+      <c r="R13" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="U13" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F13" s="7">
-        <f>F12</f>
-        <v>0.1</v>
-      </c>
-      <c r="H13" s="2">
+        <v>66.578227200000001</v>
+      </c>
+      <c r="V13" s="2">
         <f t="shared" si="7"/>
-        <v>66.578227200000001</v>
-      </c>
-      <c r="I13" s="2">
-        <f>F13*H13</f>
-        <v>6.6578227200000004</v>
-      </c>
-      <c r="K13" s="2">
-        <f>I13-D13</f>
-        <v>-1.3421772799999996</v>
-      </c>
-      <c r="L13" s="2">
-        <f t="shared" si="0"/>
-        <v>1.8014399999999999</v>
-      </c>
-      <c r="N13" s="2">
-        <f>2*F13*K13</f>
-        <v>-0.26843545599999991</v>
-      </c>
-      <c r="O13" s="2">
-        <f>E13*N13</f>
-        <v>-4.831838207999998</v>
-      </c>
-      <c r="P13" s="2">
-        <f t="shared" si="8"/>
-        <v>71.410065407999994</v>
-      </c>
-      <c r="R13" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U13" s="2">
-        <f t="shared" si="2"/>
-        <v>66.578227200000001</v>
-      </c>
-      <c r="V13" s="2">
-        <f t="shared" si="3"/>
         <v>1.8014399999999999</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="12"/>
+        <v>71.410065407999994</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1410065407999994</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.85899345920000059</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.73787000000000003</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.17179869184000013</v>
+      </c>
+      <c r="O14" s="2">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="D14" s="7">
+        <v>-3.0923764531200022</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="13"/>
+        <v>74.502441861119991</v>
+      </c>
+      <c r="R14" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F14" s="7">
-        <f>F13</f>
-        <v>0.1</v>
-      </c>
-      <c r="H14" s="2">
+        <v>71.410065407999994</v>
+      </c>
+      <c r="V14" s="2">
         <f t="shared" si="7"/>
-        <v>71.410065407999994</v>
-      </c>
-      <c r="I14" s="2">
-        <f>F14*H14</f>
-        <v>7.1410065407999994</v>
-      </c>
-      <c r="K14" s="2">
-        <f>I14-D14</f>
-        <v>-0.85899345920000059</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.73787000000000003</v>
-      </c>
-      <c r="N14" s="2">
-        <f>2*F14*K14</f>
-        <v>-0.17179869184000013</v>
-      </c>
-      <c r="O14" s="2">
-        <f>E14*N14</f>
-        <v>-3.0923764531200022</v>
-      </c>
-      <c r="P14" s="2">
-        <f t="shared" si="8"/>
-        <v>74.502441861119991</v>
-      </c>
-      <c r="R14" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U14" s="2">
-        <f t="shared" si="2"/>
-        <v>71.410065407999994</v>
-      </c>
-      <c r="V14" s="2">
-        <f t="shared" si="3"/>
         <v>0.73787000000000003</v>
       </c>
     </row>
     <row r="15" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="12"/>
+        <v>74.502441861119991</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4502441861119992</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.54975581388800077</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.30223</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.10995116277760016</v>
+      </c>
+      <c r="O15" s="2">
         <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="D15" s="7">
+        <v>-1.9791209299968029</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="13"/>
+        <v>76.481562791116787</v>
+      </c>
+      <c r="R15" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="U15" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F15" s="7">
-        <f>F14</f>
-        <v>0.1</v>
-      </c>
-      <c r="H15" s="2">
+        <v>74.502441861119991</v>
+      </c>
+      <c r="V15" s="2">
         <f t="shared" si="7"/>
-        <v>74.502441861119991</v>
-      </c>
-      <c r="I15" s="2">
-        <f>F15*H15</f>
-        <v>7.4502441861119992</v>
-      </c>
-      <c r="K15" s="2">
-        <f>I15-D15</f>
-        <v>-0.54975581388800077</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.30223</v>
-      </c>
-      <c r="N15" s="2">
-        <f>2*F15*K15</f>
-        <v>-0.10995116277760016</v>
-      </c>
-      <c r="O15" s="2">
-        <f>E15*N15</f>
-        <v>-1.9791209299968029</v>
-      </c>
-      <c r="P15" s="2">
-        <f t="shared" si="8"/>
-        <v>76.481562791116787</v>
-      </c>
-      <c r="R15" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U15" s="2">
-        <f t="shared" si="2"/>
-        <v>74.502441861119991</v>
-      </c>
-      <c r="V15" s="2">
-        <f t="shared" si="3"/>
         <v>0.30223</v>
       </c>
     </row>
     <row r="16" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="12"/>
+        <v>76.481562791116787</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>7.6481562791116788</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.35184372088832117</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>0.12379</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="3"/>
+        <v>-7.0368744177664241E-2</v>
+      </c>
+      <c r="O16" s="2">
         <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="D16" s="7">
+        <v>-1.2666373951979564</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="13"/>
+        <v>77.748200186314747</v>
+      </c>
+      <c r="R16" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="U16" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F16" s="7">
-        <f>F15</f>
-        <v>0.1</v>
-      </c>
-      <c r="H16" s="2">
+        <v>76.481562791116787</v>
+      </c>
+      <c r="V16" s="2">
         <f t="shared" si="7"/>
-        <v>76.481562791116787</v>
-      </c>
-      <c r="I16" s="2">
-        <f>F16*H16</f>
-        <v>7.6481562791116788</v>
-      </c>
-      <c r="K16" s="2">
-        <f>I16-D16</f>
-        <v>-0.35184372088832117</v>
-      </c>
-      <c r="L16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.12379</v>
-      </c>
-      <c r="N16" s="2">
-        <f>2*F16*K16</f>
-        <v>-7.0368744177664241E-2</v>
-      </c>
-      <c r="O16" s="2">
-        <f>E16*N16</f>
-        <v>-1.2666373951979564</v>
-      </c>
-      <c r="P16" s="2">
-        <f t="shared" si="8"/>
-        <v>77.748200186314747</v>
-      </c>
-      <c r="R16" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U16" s="2">
-        <f t="shared" si="2"/>
-        <v>76.481562791116787</v>
-      </c>
-      <c r="V16" s="2">
-        <f t="shared" si="3"/>
         <v>0.12379</v>
       </c>
     </row>
     <row r="17" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="12"/>
+        <v>77.748200186314747</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>7.7748200186314751</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.22517998136852491</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>5.0709999999999998E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="3"/>
+        <v>-4.5035996273704984E-2</v>
+      </c>
+      <c r="O17" s="2">
         <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="D17" s="7">
+        <v>-0.81064793292668968</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="13"/>
+        <v>78.558848119241432</v>
+      </c>
+      <c r="R17" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="U17" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F17" s="7">
-        <f>F16</f>
-        <v>0.1</v>
-      </c>
-      <c r="H17" s="2">
+        <v>77.748200186314747</v>
+      </c>
+      <c r="V17" s="2">
         <f t="shared" si="7"/>
-        <v>77.748200186314747</v>
-      </c>
-      <c r="I17" s="2">
-        <f>F17*H17</f>
-        <v>7.7748200186314751</v>
-      </c>
-      <c r="K17" s="2">
-        <f>I17-D17</f>
-        <v>-0.22517998136852491</v>
-      </c>
-      <c r="L17" s="2">
-        <f t="shared" si="0"/>
-        <v>5.0709999999999998E-2</v>
-      </c>
-      <c r="N17" s="2">
-        <f>2*F17*K17</f>
-        <v>-4.5035996273704984E-2</v>
-      </c>
-      <c r="O17" s="2">
-        <f>E17*N17</f>
-        <v>-0.81064793292668968</v>
-      </c>
-      <c r="P17" s="2">
-        <f t="shared" si="8"/>
-        <v>78.558848119241432</v>
-      </c>
-      <c r="R17" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U17" s="2">
-        <f t="shared" si="2"/>
-        <v>77.748200186314747</v>
-      </c>
-      <c r="V17" s="2">
-        <f t="shared" si="3"/>
         <v>5.0709999999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F18" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="12"/>
+        <v>78.558848119241432</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>7.8558848119241436</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.14411518807585644</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>2.077E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="3"/>
+        <v>-2.8823037615171288E-2</v>
+      </c>
+      <c r="O18" s="2">
         <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="D18" s="7">
+        <v>-0.51881467707308315</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="13"/>
+        <v>79.077662796314513</v>
+      </c>
+      <c r="R18" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="U18" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F18" s="7">
-        <f>F17</f>
-        <v>0.1</v>
-      </c>
-      <c r="H18" s="2">
+        <v>78.558848119241432</v>
+      </c>
+      <c r="V18" s="2">
         <f t="shared" si="7"/>
-        <v>78.558848119241432</v>
-      </c>
-      <c r="I18" s="2">
-        <f>F18*H18</f>
-        <v>7.8558848119241436</v>
-      </c>
-      <c r="K18" s="2">
-        <f>I18-D18</f>
-        <v>-0.14411518807585644</v>
-      </c>
-      <c r="L18" s="2">
-        <f t="shared" si="0"/>
-        <v>2.077E-2</v>
-      </c>
-      <c r="N18" s="2">
-        <f>2*F18*K18</f>
-        <v>-2.8823037615171288E-2</v>
-      </c>
-      <c r="O18" s="2">
-        <f>E18*N18</f>
-        <v>-0.51881467707308315</v>
-      </c>
-      <c r="P18" s="2">
-        <f t="shared" si="8"/>
-        <v>79.077662796314513</v>
-      </c>
-      <c r="R18" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U18" s="2">
-        <f t="shared" si="2"/>
-        <v>78.558848119241432</v>
-      </c>
-      <c r="V18" s="2">
-        <f t="shared" si="3"/>
         <v>2.077E-2</v>
       </c>
     </row>
     <row r="19" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F19" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="12"/>
+        <v>79.077662796314513</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9077662796314518</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="1"/>
+        <v>-9.2233720368548155E-2</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5100000000000002E-3</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.8446744073709633E-2</v>
+      </c>
+      <c r="O19" s="2">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="D19" s="7">
+        <v>-0.3320413933267734</v>
+      </c>
+      <c r="P19" s="2">
+        <f t="shared" si="13"/>
+        <v>79.409704189641289</v>
+      </c>
+      <c r="R19" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="U19" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F19" s="7">
-        <f>F18</f>
-        <v>0.1</v>
-      </c>
-      <c r="H19" s="2">
+        <v>79.077662796314513</v>
+      </c>
+      <c r="V19" s="2">
         <f t="shared" si="7"/>
-        <v>79.077662796314513</v>
-      </c>
-      <c r="I19" s="2">
-        <f>F19*H19</f>
-        <v>7.9077662796314518</v>
-      </c>
-      <c r="K19" s="2">
-        <f>I19-D19</f>
-        <v>-9.2233720368548155E-2</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="0"/>
-        <v>8.5100000000000002E-3</v>
-      </c>
-      <c r="N19" s="2">
-        <f>2*F19*K19</f>
-        <v>-1.8446744073709633E-2</v>
-      </c>
-      <c r="O19" s="2">
-        <f>E19*N19</f>
-        <v>-0.3320413933267734</v>
-      </c>
-      <c r="P19" s="2">
-        <f t="shared" si="8"/>
-        <v>79.409704189641289</v>
-      </c>
-      <c r="R19" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U19" s="2">
-        <f t="shared" si="2"/>
-        <v>79.077662796314513</v>
-      </c>
-      <c r="V19" s="2">
-        <f t="shared" si="3"/>
         <v>8.5100000000000002E-3</v>
       </c>
     </row>
     <row r="20" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="12"/>
+        <v>79.409704189641289</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9409704189641293</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.9029581035870748E-2</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>3.48E-3</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.1805916207174151E-2</v>
+      </c>
+      <c r="O20" s="2">
         <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="D20" s="7">
+        <v>-0.21250649172913472</v>
+      </c>
+      <c r="P20" s="2">
+        <f t="shared" si="13"/>
+        <v>79.622210681370419</v>
+      </c>
+      <c r="R20" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="U20" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F20" s="7">
-        <f>F19</f>
-        <v>0.1</v>
-      </c>
-      <c r="H20" s="2">
+        <v>79.409704189641289</v>
+      </c>
+      <c r="V20" s="2">
         <f t="shared" si="7"/>
-        <v>79.409704189641289</v>
-      </c>
-      <c r="I20" s="2">
-        <f>F20*H20</f>
-        <v>7.9409704189641293</v>
-      </c>
-      <c r="K20" s="2">
-        <f>I20-D20</f>
-        <v>-5.9029581035870748E-2</v>
-      </c>
-      <c r="L20" s="2">
-        <f t="shared" si="0"/>
-        <v>3.48E-3</v>
-      </c>
-      <c r="N20" s="2">
-        <f>2*F20*K20</f>
-        <v>-1.1805916207174151E-2</v>
-      </c>
-      <c r="O20" s="2">
-        <f>E20*N20</f>
-        <v>-0.21250649172913472</v>
-      </c>
-      <c r="P20" s="2">
-        <f t="shared" si="8"/>
-        <v>79.622210681370419</v>
-      </c>
-      <c r="R20" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U20" s="2">
-        <f t="shared" si="2"/>
-        <v>79.409704189641289</v>
-      </c>
-      <c r="V20" s="2">
-        <f t="shared" si="3"/>
         <v>3.48E-3</v>
       </c>
     </row>
     <row r="21" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="12"/>
+        <v>79.622210681370419</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9622210681370422</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.7778931862957776E-2</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4300000000000001E-3</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="3"/>
+        <v>-7.5557863725915558E-3</v>
+      </c>
+      <c r="O21" s="2">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="D21" s="7">
+        <v>-0.13600415470664801</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="13"/>
+        <v>79.758214836077073</v>
+      </c>
+      <c r="R21" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="U21" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F21" s="7">
-        <f>F20</f>
-        <v>0.1</v>
-      </c>
-      <c r="H21" s="2">
+        <v>79.622210681370419</v>
+      </c>
+      <c r="V21" s="2">
         <f t="shared" si="7"/>
-        <v>79.622210681370419</v>
-      </c>
-      <c r="I21" s="2">
-        <f>F21*H21</f>
-        <v>7.9622210681370422</v>
-      </c>
-      <c r="K21" s="2">
-        <f>I21-D21</f>
-        <v>-3.7778931862957776E-2</v>
-      </c>
-      <c r="L21" s="2">
-        <f t="shared" si="0"/>
-        <v>1.4300000000000001E-3</v>
-      </c>
-      <c r="N21" s="2">
-        <f>2*F21*K21</f>
-        <v>-7.5557863725915558E-3</v>
-      </c>
-      <c r="O21" s="2">
-        <f>E21*N21</f>
-        <v>-0.13600415470664801</v>
-      </c>
-      <c r="P21" s="2">
-        <f t="shared" si="8"/>
-        <v>79.758214836077073</v>
-      </c>
-      <c r="R21" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U21" s="2">
-        <f t="shared" si="2"/>
-        <v>79.622210681370419</v>
-      </c>
-      <c r="V21" s="2">
-        <f t="shared" si="3"/>
         <v>1.4300000000000001E-3</v>
       </c>
     </row>
     <row r="22" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="11"/>
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="12"/>
+        <v>79.758214836077073</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9758214836077075</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.4178516392292515E-2</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="2"/>
+        <v>5.8E-4</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="3"/>
+        <v>-4.835703278458503E-3</v>
+      </c>
+      <c r="O22" s="2">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="D22" s="7">
+        <v>-8.7042659012253054E-2</v>
+      </c>
+      <c r="P22" s="2">
+        <f t="shared" si="13"/>
+        <v>79.845257495089328</v>
+      </c>
+      <c r="R22" s="7" t="b">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="U22" s="2">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="F22" s="7">
-        <f>F21</f>
-        <v>0.1</v>
-      </c>
-      <c r="H22" s="2">
+        <v>79.758214836077073</v>
+      </c>
+      <c r="V22" s="2">
         <f t="shared" si="7"/>
-        <v>79.758214836077073</v>
-      </c>
-      <c r="I22" s="2">
-        <f>F22*H22</f>
-        <v>7.9758214836077075</v>
-      </c>
-      <c r="K22" s="2">
-        <f>I22-D22</f>
-        <v>-2.4178516392292515E-2</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" si="0"/>
-        <v>5.8E-4</v>
-      </c>
-      <c r="N22" s="2">
-        <f>2*F22*K22</f>
-        <v>-4.835703278458503E-3</v>
-      </c>
-      <c r="O22" s="2">
-        <f>E22*N22</f>
-        <v>-8.7042659012253054E-2</v>
-      </c>
-      <c r="P22" s="2">
-        <f t="shared" si="8"/>
-        <v>79.845257495089328</v>
-      </c>
-      <c r="R22" s="7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U22" s="2">
-        <f t="shared" si="2"/>
-        <v>79.758214836077073</v>
-      </c>
-      <c r="V22" s="2">
-        <f t="shared" si="3"/>
         <v>5.8E-4</v>
       </c>
     </row>
     <row r="23" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
-        <f t="shared" ref="B23:B25" si="9">B22+1</f>
+        <f t="shared" ref="B23:B25" si="14">B22+1</f>
         <v>15</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" ref="D23:D25" si="10">D22</f>
+        <f t="shared" ref="D23:D25" si="15">D22</f>
         <v>8</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" ref="E23:E25" si="11">E22</f>
+        <f t="shared" ref="E23:E25" si="16">E22</f>
         <v>18</v>
       </c>
       <c r="F23" s="7">
-        <f>F22</f>
+        <f t="shared" si="11"/>
         <v>0.1</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" ref="H23:H25" si="12">P22</f>
+        <f t="shared" ref="H23:H25" si="17">P22</f>
         <v>79.845257495089328</v>
       </c>
       <c r="I23" s="2">
-        <f>F23*H23</f>
+        <f t="shared" si="0"/>
         <v>7.9845257495089328</v>
       </c>
       <c r="K23" s="2">
-        <f>I23-D23</f>
+        <f t="shared" si="1"/>
         <v>-1.547425049106721E-2</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.4000000000000001E-4</v>
       </c>
       <c r="N23" s="2">
-        <f>2*F23*K23</f>
+        <f t="shared" si="3"/>
         <v>-3.0948500982134423E-3</v>
       </c>
       <c r="O23" s="2">
-        <f>E23*N23</f>
+        <f t="shared" si="4"/>
         <v>-5.5707301767841957E-2</v>
       </c>
       <c r="P23" s="2">
-        <f t="shared" ref="P23:P25" si="13">H23-O23</f>
+        <f t="shared" ref="P23:P25" si="18">H23-O23</f>
         <v>79.900964796857167</v>
       </c>
       <c r="R23" s="7" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>79.845257495089328</v>
       </c>
       <c r="V23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.4000000000000001E-4</v>
       </c>
     </row>
     <row r="24" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>16</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="E24" s="7">
+        <f t="shared" si="16"/>
+        <v>18</v>
+      </c>
+      <c r="F24" s="7">
         <f t="shared" si="11"/>
-        <v>18</v>
-      </c>
-      <c r="F24" s="7">
-        <f>F23</f>
         <v>0.1</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>79.900964796857167</v>
       </c>
       <c r="I24" s="2">
-        <f>F24*H24</f>
+        <f t="shared" si="0"/>
         <v>7.9900964796857172</v>
       </c>
       <c r="K24" s="2">
-        <f>I24-D24</f>
+        <f t="shared" si="1"/>
         <v>-9.9035203142827655E-3</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1E-4</v>
       </c>
       <c r="N24" s="2">
-        <f>2*F24*K24</f>
+        <f t="shared" si="3"/>
         <v>-1.9807040628565531E-3</v>
       </c>
       <c r="O24" s="2">
-        <f>E24*N24</f>
+        <f t="shared" si="4"/>
         <v>-3.5652673131417956E-2</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>79.93661746998859</v>
       </c>
       <c r="R24" s="7" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>79.900964796857167</v>
       </c>
       <c r="V24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1E-4</v>
       </c>
     </row>
     <row r="25" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>17</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="E25" s="7">
+        <f t="shared" si="16"/>
+        <v>18</v>
+      </c>
+      <c r="F25" s="7">
         <f t="shared" si="11"/>
-        <v>18</v>
-      </c>
-      <c r="F25" s="7">
-        <f>F24</f>
         <v>0.1</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>79.93661746998859</v>
       </c>
       <c r="I25" s="2">
-        <f>F25*H25</f>
+        <f t="shared" si="0"/>
         <v>7.9936617469988596</v>
       </c>
       <c r="K25" s="2">
-        <f>I25-D25</f>
+        <f t="shared" si="1"/>
         <v>-6.338253001140437E-3</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="N25" s="2">
-        <f>2*F25*K25</f>
+        <f t="shared" si="3"/>
         <v>-1.2676506002280874E-3</v>
       </c>
       <c r="O25" s="2">
-        <f>E25*N25</f>
+        <f t="shared" si="4"/>
         <v>-2.2817710804105575E-2</v>
       </c>
       <c r="P25" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>79.959435180792696</v>
       </c>
       <c r="R25" s="7" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>79.93661746998859</v>
       </c>
       <c r="V25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
     <row r="26" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
-        <f t="shared" ref="B26" si="14">B25+1</f>
+        <f t="shared" ref="B26" si="19">B25+1</f>
         <v>18</v>
       </c>
       <c r="D26" s="7">
-        <f t="shared" ref="D26" si="15">D25</f>
+        <f t="shared" ref="D26" si="20">D25</f>
         <v>8</v>
       </c>
       <c r="E26" s="7">
-        <f t="shared" ref="E26" si="16">E25</f>
+        <f t="shared" ref="E26" si="21">E25</f>
         <v>18</v>
       </c>
       <c r="F26" s="7">
-        <f>F25</f>
+        <f t="shared" si="11"/>
         <v>0.1</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ref="H26" si="17">P25</f>
+        <f t="shared" ref="H26" si="22">P25</f>
         <v>79.959435180792696</v>
       </c>
       <c r="I26" s="2">
-        <f>F26*H26</f>
+        <f t="shared" si="0"/>
         <v>7.9959435180792697</v>
       </c>
       <c r="K26" s="2">
-        <f>I26-D26</f>
+        <f t="shared" si="1"/>
         <v>-4.0564819207302705E-3</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="N26" s="2">
-        <f>2*F26*K26</f>
+        <f t="shared" si="3"/>
         <v>-8.1129638414605414E-4</v>
       </c>
       <c r="O26" s="2">
-        <f>E26*N26</f>
+        <f t="shared" si="4"/>
         <v>-1.4603334914628974E-2</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" ref="P26" si="18">H26-O26</f>
+        <f t="shared" ref="P26" si="23">H26-O26</f>
         <v>79.974038515707321</v>
       </c>
       <c r="R26" s="7" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U26" s="2">
-        <f t="shared" ref="U26" si="19">H26</f>
+        <f t="shared" ref="U26" si="24">H26</f>
         <v>79.959435180792696</v>
       </c>
       <c r="V26" s="2">
-        <f t="shared" ref="V26" si="20">L26</f>
+        <f t="shared" ref="V26" si="25">L26</f>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="27" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
-        <f t="shared" ref="B27:B28" si="21">B26+1</f>
+        <f t="shared" ref="B27:B28" si="26">B26+1</f>
         <v>19</v>
       </c>
       <c r="D27" s="7">
-        <f t="shared" ref="D27:D28" si="22">D26</f>
+        <f t="shared" ref="D27:D28" si="27">D26</f>
         <v>8</v>
       </c>
       <c r="E27" s="7">
-        <f t="shared" ref="E27:E28" si="23">E26</f>
+        <f t="shared" ref="E27:E28" si="28">E26</f>
         <v>18</v>
       </c>
       <c r="F27" s="7">
-        <f>F26</f>
+        <f t="shared" si="11"/>
         <v>0.1</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ref="H27:H28" si="24">P26</f>
+        <f t="shared" ref="H27:H28" si="29">P26</f>
         <v>79.974038515707321</v>
       </c>
       <c r="I27" s="2">
-        <f>F27*H27</f>
+        <f t="shared" si="0"/>
         <v>7.9974038515707324</v>
       </c>
       <c r="K27" s="2">
-        <f>I27-D27</f>
+        <f t="shared" si="1"/>
         <v>-2.5961484292675863E-3</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="N27" s="2">
-        <f>2*F27*K27</f>
+        <f t="shared" si="3"/>
         <v>-5.1922968585351727E-4</v>
       </c>
       <c r="O27" s="2">
-        <f>E27*N27</f>
+        <f t="shared" si="4"/>
         <v>-9.3461343453633116E-3</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" ref="P27:P28" si="25">H27-O27</f>
+        <f t="shared" ref="P27:P28" si="30">H27-O27</f>
         <v>79.983384650052685</v>
       </c>
       <c r="R27" s="7" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U27" s="2">
-        <f t="shared" ref="U27:U28" si="26">H27</f>
+        <f t="shared" ref="U27:U28" si="31">H27</f>
         <v>79.974038515707321</v>
       </c>
       <c r="V27" s="2">
-        <f t="shared" ref="V27:V28" si="27">L27</f>
+        <f t="shared" ref="V27:V28" si="32">L27</f>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="28" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="D28" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>8</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>18</v>
       </c>
       <c r="F28" s="7">
-        <f>F27</f>
+        <f t="shared" si="11"/>
         <v>0.1</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>79.983384650052685</v>
       </c>
       <c r="I28" s="2">
-        <f>F28*H28</f>
+        <f t="shared" si="0"/>
         <v>7.9983384650052685</v>
       </c>
       <c r="K28" s="2">
-        <f>I28-D28</f>
+        <f t="shared" si="1"/>
         <v>-1.6615349947315394E-3</v>
       </c>
       <c r="L28" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N28" s="2">
-        <f>2*F28*K28</f>
+        <f t="shared" si="3"/>
         <v>-3.3230699894630793E-4</v>
       </c>
       <c r="O28" s="2">
-        <f>E28*N28</f>
+        <f t="shared" si="4"/>
         <v>-5.9815259810335423E-3</v>
       </c>
       <c r="P28" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>79.989366176033712</v>
       </c>
-      <c r="R28" s="27" t="b">
-        <f t="shared" si="1"/>
+      <c r="R28" s="17" t="b">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U28" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>79.983384650052685</v>
       </c>
       <c r="V28" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -6804,38 +6800,38 @@
       <c r="R31" s="9"/>
     </row>
     <row r="32" spans="2:22" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="25"/>
-      <c r="F32" s="21"/>
-      <c r="H32" s="18" t="s">
+      <c r="F32" s="26"/>
+      <c r="H32" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="18"/>
-      <c r="K32" s="20" t="s">
+      <c r="I32" s="23"/>
+      <c r="K32" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L32" s="21"/>
-      <c r="N32" s="18" t="s">
+      <c r="L32" s="26"/>
+      <c r="N32" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="R32" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="U32" s="19" t="s">
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="R32" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="U32" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="V32" s="19"/>
+      <c r="V32" s="27"/>
     </row>
     <row r="33" spans="2:22" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="23"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="6"/>
       <c r="D33" s="13" t="s">
         <v>5</v>
@@ -6867,7 +6863,7 @@
       <c r="P33" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="R33" s="23"/>
+      <c r="R33" s="20"/>
       <c r="U33" s="4" t="str">
         <f>H33</f>
         <v>Weight</v>
@@ -6878,7 +6874,7 @@
       </c>
     </row>
     <row r="34" spans="2:22" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="17"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="6"/>
       <c r="D34" s="14" t="s">
         <v>31</v>
@@ -6915,7 +6911,7 @@
       </c>
       <c r="Q34" s="15"/>
       <c r="R34" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
@@ -6937,23 +6933,23 @@
         <v>160</v>
       </c>
       <c r="I35" s="2">
-        <f>F35*H35</f>
+        <f t="shared" ref="I35:I54" si="33">F35*H35</f>
         <v>16</v>
       </c>
       <c r="K35" s="2">
-        <f>I35-D35</f>
+        <f t="shared" ref="K35:K54" si="34">I35-D35</f>
         <v>8</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" ref="L35:L37" si="28">ROUND(POWER(K35,2), 5)</f>
+        <f t="shared" ref="L35:L37" si="35">ROUND(POWER(K35,2), 5)</f>
         <v>64</v>
       </c>
       <c r="N35" s="2">
-        <f>2*F35*K35</f>
+        <f t="shared" ref="N35:N54" si="36">2*F35*K35</f>
         <v>1.6</v>
       </c>
       <c r="O35" s="2">
-        <f>E35*N35</f>
+        <f t="shared" ref="O35:O54" si="37">E35*N35</f>
         <v>28.8</v>
       </c>
       <c r="P35" s="2">
@@ -6995,23 +6991,23 @@
         <v>131.19999999999999</v>
       </c>
       <c r="I36" s="2">
-        <f>F36*H36</f>
+        <f t="shared" si="33"/>
         <v>13.12</v>
       </c>
       <c r="K36" s="2">
-        <f>I36-D36</f>
+        <f t="shared" si="34"/>
         <v>5.1199999999999992</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>26.214400000000001</v>
       </c>
       <c r="N36" s="2">
-        <f>2*F36*K36</f>
+        <f t="shared" si="36"/>
         <v>1.0239999999999998</v>
       </c>
       <c r="O36" s="2">
-        <f>E36*N36</f>
+        <f t="shared" si="37"/>
         <v>18.431999999999995</v>
       </c>
       <c r="P36" s="2">
@@ -7019,103 +7015,103 @@
         <v>112.768</v>
       </c>
       <c r="R36" s="7" t="b">
-        <f t="shared" ref="R36:R54" si="29">(L36&lt;&gt;0)</f>
+        <f t="shared" ref="R36:R54" si="38">(L36&lt;&gt;0)</f>
         <v>1</v>
       </c>
       <c r="U36" s="2">
-        <f t="shared" ref="U36:U50" si="30">H36</f>
+        <f t="shared" ref="U36:U50" si="39">H36</f>
         <v>131.19999999999999</v>
       </c>
       <c r="V36" s="2">
-        <f t="shared" ref="V36:V50" si="31">L36</f>
+        <f t="shared" ref="V36:V50" si="40">L36</f>
         <v>26.214400000000001</v>
       </c>
     </row>
     <row r="37" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7">
-        <f t="shared" ref="B37:B50" si="32">B36+1</f>
+        <f t="shared" ref="B37:B50" si="41">B36+1</f>
         <v>3</v>
       </c>
       <c r="D37" s="7">
-        <f t="shared" ref="D37:D50" si="33">D36</f>
+        <f t="shared" ref="D37:D50" si="42">D36</f>
         <v>8</v>
       </c>
       <c r="E37" s="7">
-        <f t="shared" ref="E37:E50" si="34">E36</f>
+        <f t="shared" ref="E37:E50" si="43">E36</f>
         <v>18</v>
       </c>
       <c r="F37" s="7">
-        <f>F36</f>
+        <f t="shared" ref="F37:F54" si="44">F36</f>
         <v>0.1</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" ref="H37:H50" si="35">P36</f>
+        <f t="shared" ref="H37:H50" si="45">P36</f>
         <v>112.768</v>
       </c>
       <c r="I37" s="2">
-        <f>F37*H37</f>
+        <f t="shared" si="33"/>
         <v>11.276800000000001</v>
       </c>
       <c r="K37" s="2">
-        <f>I37-D37</f>
+        <f t="shared" si="34"/>
         <v>3.2768000000000015</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="35"/>
         <v>10.73742</v>
       </c>
       <c r="N37" s="2">
-        <f>2*F37*K37</f>
+        <f t="shared" si="36"/>
         <v>0.65536000000000039</v>
       </c>
       <c r="O37" s="2">
-        <f>E37*N37</f>
+        <f t="shared" si="37"/>
         <v>11.796480000000006</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" ref="P37:P50" si="36">H37-O37</f>
+        <f t="shared" ref="P37:P50" si="46">H37-O37</f>
         <v>100.97152</v>
       </c>
       <c r="R37" s="7" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="U37" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="39"/>
         <v>112.768</v>
       </c>
       <c r="V37" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>10.73742</v>
       </c>
     </row>
     <row r="38" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>4</v>
       </c>
       <c r="D38" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E38" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F38" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="45"/>
+        <v>100.97152</v>
+      </c>
+      <c r="I38" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E38" s="7">
+        <v>10.097152000000001</v>
+      </c>
+      <c r="K38" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F38" s="7">
-        <f>F37</f>
-        <v>0.1</v>
-      </c>
-      <c r="H38" s="2">
-        <f t="shared" si="35"/>
-        <v>100.97152</v>
-      </c>
-      <c r="I38" s="2">
-        <f>F38*H38</f>
-        <v>10.097152000000001</v>
-      </c>
-      <c r="K38" s="2">
-        <f>I38-D38</f>
         <v>2.0971520000000012</v>
       </c>
       <c r="L38" s="2">
@@ -7123,977 +7119,977 @@
         <v>4.3980499999999996</v>
       </c>
       <c r="N38" s="2">
-        <f>2*F38*K38</f>
+        <f t="shared" si="36"/>
         <v>0.41943040000000026</v>
       </c>
       <c r="O38" s="2">
-        <f>E38*N38</f>
+        <f t="shared" si="37"/>
         <v>7.549747200000005</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="46"/>
         <v>93.421772799999999</v>
       </c>
       <c r="R38" s="7" t="b">
-        <f t="shared" si="29"/>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="U38" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="39"/>
         <v>100.97152</v>
       </c>
       <c r="V38" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>4.3980499999999996</v>
       </c>
     </row>
     <row r="39" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>5</v>
       </c>
       <c r="D39" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E39" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="45"/>
+        <v>93.421772799999999</v>
+      </c>
+      <c r="I39" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E39" s="7">
+        <v>9.3421772799999996</v>
+      </c>
+      <c r="K39" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F39" s="7">
-        <f>F38</f>
-        <v>0.1</v>
-      </c>
-      <c r="H39" s="2">
-        <f t="shared" si="35"/>
+        <v>1.3421772799999996</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" ref="L39:L40" si="47">ROUND(POWER(K39,2), 5)</f>
+        <v>1.8014399999999999</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="36"/>
+        <v>0.26843545599999991</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="37"/>
+        <v>4.831838207999998</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="46"/>
+        <v>88.589934592000006</v>
+      </c>
+      <c r="R39" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U39" s="2">
+        <f t="shared" si="39"/>
         <v>93.421772799999999</v>
       </c>
-      <c r="I39" s="2">
-        <f>F39*H39</f>
-        <v>9.3421772799999996</v>
-      </c>
-      <c r="K39" s="2">
-        <f>I39-D39</f>
-        <v>1.3421772799999996</v>
-      </c>
-      <c r="L39" s="2">
-        <f t="shared" ref="L39:L40" si="37">ROUND(POWER(K39,2), 5)</f>
-        <v>1.8014399999999999</v>
-      </c>
-      <c r="N39" s="2">
-        <f>2*F39*K39</f>
-        <v>0.26843545599999991</v>
-      </c>
-      <c r="O39" s="2">
-        <f>E39*N39</f>
-        <v>4.831838207999998</v>
-      </c>
-      <c r="P39" s="2">
-        <f t="shared" si="36"/>
-        <v>88.589934592000006</v>
-      </c>
-      <c r="R39" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U39" s="2">
-        <f t="shared" si="30"/>
-        <v>93.421772799999999</v>
-      </c>
       <c r="V39" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>1.8014399999999999</v>
       </c>
     </row>
     <row r="40" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>6</v>
       </c>
       <c r="D40" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E40" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F40" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="45"/>
+        <v>88.589934592000006</v>
+      </c>
+      <c r="I40" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E40" s="7">
+        <v>8.8589934592000006</v>
+      </c>
+      <c r="K40" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F40" s="7">
-        <f>F39</f>
-        <v>0.1</v>
-      </c>
-      <c r="H40" s="2">
-        <f t="shared" si="35"/>
+        <v>0.85899345920000059</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="47"/>
+        <v>0.73787000000000003</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="36"/>
+        <v>0.17179869184000013</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="37"/>
+        <v>3.0923764531200022</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="46"/>
+        <v>85.497558138880009</v>
+      </c>
+      <c r="R40" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U40" s="2">
+        <f t="shared" si="39"/>
         <v>88.589934592000006</v>
       </c>
-      <c r="I40" s="2">
-        <f>F40*H40</f>
-        <v>8.8589934592000006</v>
-      </c>
-      <c r="K40" s="2">
-        <f>I40-D40</f>
-        <v>0.85899345920000059</v>
-      </c>
-      <c r="L40" s="2">
-        <f t="shared" si="37"/>
-        <v>0.73787000000000003</v>
-      </c>
-      <c r="N40" s="2">
-        <f>2*F40*K40</f>
-        <v>0.17179869184000013</v>
-      </c>
-      <c r="O40" s="2">
-        <f>E40*N40</f>
-        <v>3.0923764531200022</v>
-      </c>
-      <c r="P40" s="2">
-        <f t="shared" si="36"/>
-        <v>85.497558138880009</v>
-      </c>
-      <c r="R40" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U40" s="2">
-        <f t="shared" si="30"/>
-        <v>88.589934592000006</v>
-      </c>
       <c r="V40" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>0.73787000000000003</v>
       </c>
     </row>
     <row r="41" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="D41" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F41" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="45"/>
+        <v>85.497558138880009</v>
+      </c>
+      <c r="I41" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E41" s="7">
+        <v>8.5497558138880017</v>
+      </c>
+      <c r="K41" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F41" s="7">
-        <f>F40</f>
-        <v>0.1</v>
-      </c>
-      <c r="H41" s="2">
-        <f t="shared" si="35"/>
+        <v>0.54975581388800165</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" ref="L41:L54" si="48">ROUND(POWER(K41,2), 5)</f>
+        <v>0.30223</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="36"/>
+        <v>0.10995116277760034</v>
+      </c>
+      <c r="O41" s="2">
+        <f t="shared" si="37"/>
+        <v>1.979120929996806</v>
+      </c>
+      <c r="P41" s="2">
+        <f t="shared" si="46"/>
+        <v>83.518437208883199</v>
+      </c>
+      <c r="R41" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U41" s="2">
+        <f t="shared" si="39"/>
         <v>85.497558138880009</v>
       </c>
-      <c r="I41" s="2">
-        <f>F41*H41</f>
-        <v>8.5497558138880017</v>
-      </c>
-      <c r="K41" s="2">
-        <f>I41-D41</f>
-        <v>0.54975581388800165</v>
-      </c>
-      <c r="L41" s="2">
-        <f t="shared" ref="L41:L54" si="38">ROUND(POWER(K41,2), 5)</f>
-        <v>0.30223</v>
-      </c>
-      <c r="N41" s="2">
-        <f>2*F41*K41</f>
-        <v>0.10995116277760034</v>
-      </c>
-      <c r="O41" s="2">
-        <f>E41*N41</f>
-        <v>1.979120929996806</v>
-      </c>
-      <c r="P41" s="2">
-        <f t="shared" si="36"/>
-        <v>83.518437208883199</v>
-      </c>
-      <c r="R41" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U41" s="2">
-        <f t="shared" si="30"/>
-        <v>85.497558138880009</v>
-      </c>
       <c r="V41" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>0.30223</v>
       </c>
     </row>
     <row r="42" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>8</v>
       </c>
       <c r="D42" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E42" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F42" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="45"/>
+        <v>83.518437208883199</v>
+      </c>
+      <c r="I42" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E42" s="7">
+        <v>8.3518437208883203</v>
+      </c>
+      <c r="K42" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F42" s="7">
-        <f>F41</f>
-        <v>0.1</v>
-      </c>
-      <c r="H42" s="2">
-        <f t="shared" si="35"/>
+        <v>0.35184372088832028</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" si="48"/>
+        <v>0.12379</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="36"/>
+        <v>7.0368744177664061E-2</v>
+      </c>
+      <c r="O42" s="2">
+        <f t="shared" si="37"/>
+        <v>1.266637395197953</v>
+      </c>
+      <c r="P42" s="2">
+        <f t="shared" si="46"/>
+        <v>82.251799813685253</v>
+      </c>
+      <c r="R42" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U42" s="2">
+        <f t="shared" si="39"/>
         <v>83.518437208883199</v>
       </c>
-      <c r="I42" s="2">
-        <f>F42*H42</f>
-        <v>8.3518437208883203</v>
-      </c>
-      <c r="K42" s="2">
-        <f>I42-D42</f>
-        <v>0.35184372088832028</v>
-      </c>
-      <c r="L42" s="2">
-        <f t="shared" si="38"/>
-        <v>0.12379</v>
-      </c>
-      <c r="N42" s="2">
-        <f>2*F42*K42</f>
-        <v>7.0368744177664061E-2</v>
-      </c>
-      <c r="O42" s="2">
-        <f>E42*N42</f>
-        <v>1.266637395197953</v>
-      </c>
-      <c r="P42" s="2">
-        <f t="shared" si="36"/>
-        <v>82.251799813685253</v>
-      </c>
-      <c r="R42" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U42" s="2">
-        <f t="shared" si="30"/>
-        <v>83.518437208883199</v>
-      </c>
       <c r="V42" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>0.12379</v>
       </c>
     </row>
     <row r="43" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>9</v>
       </c>
       <c r="D43" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E43" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F43" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="45"/>
+        <v>82.251799813685253</v>
+      </c>
+      <c r="I43" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E43" s="7">
+        <v>8.2251799813685249</v>
+      </c>
+      <c r="K43" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F43" s="7">
-        <f>F42</f>
-        <v>0.1</v>
-      </c>
-      <c r="H43" s="2">
-        <f t="shared" si="35"/>
+        <v>0.22517998136852491</v>
+      </c>
+      <c r="L43" s="2">
+        <f t="shared" si="48"/>
+        <v>5.0709999999999998E-2</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="36"/>
+        <v>4.5035996273704984E-2</v>
+      </c>
+      <c r="O43" s="2">
+        <f t="shared" si="37"/>
+        <v>0.81064793292668968</v>
+      </c>
+      <c r="P43" s="2">
+        <f t="shared" si="46"/>
+        <v>81.441151880758568</v>
+      </c>
+      <c r="R43" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U43" s="2">
+        <f t="shared" si="39"/>
         <v>82.251799813685253</v>
       </c>
-      <c r="I43" s="2">
-        <f>F43*H43</f>
-        <v>8.2251799813685249</v>
-      </c>
-      <c r="K43" s="2">
-        <f>I43-D43</f>
-        <v>0.22517998136852491</v>
-      </c>
-      <c r="L43" s="2">
-        <f t="shared" si="38"/>
-        <v>5.0709999999999998E-2</v>
-      </c>
-      <c r="N43" s="2">
-        <f>2*F43*K43</f>
-        <v>4.5035996273704984E-2</v>
-      </c>
-      <c r="O43" s="2">
-        <f>E43*N43</f>
-        <v>0.81064793292668968</v>
-      </c>
-      <c r="P43" s="2">
-        <f t="shared" si="36"/>
-        <v>81.441151880758568</v>
-      </c>
-      <c r="R43" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U43" s="2">
-        <f t="shared" si="30"/>
-        <v>82.251799813685253</v>
-      </c>
       <c r="V43" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>5.0709999999999998E-2</v>
       </c>
     </row>
     <row r="44" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>10</v>
       </c>
       <c r="D44" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E44" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F44" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="45"/>
+        <v>81.441151880758568</v>
+      </c>
+      <c r="I44" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E44" s="7">
+        <v>8.1441151880758564</v>
+      </c>
+      <c r="K44" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F44" s="7">
-        <f>F43</f>
-        <v>0.1</v>
-      </c>
-      <c r="H44" s="2">
-        <f t="shared" si="35"/>
+        <v>0.14411518807585644</v>
+      </c>
+      <c r="L44" s="2">
+        <f t="shared" si="48"/>
+        <v>2.077E-2</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="36"/>
+        <v>2.8823037615171288E-2</v>
+      </c>
+      <c r="O44" s="2">
+        <f t="shared" si="37"/>
+        <v>0.51881467707308315</v>
+      </c>
+      <c r="P44" s="2">
+        <f t="shared" si="46"/>
+        <v>80.922337203685487</v>
+      </c>
+      <c r="R44" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U44" s="2">
+        <f t="shared" si="39"/>
         <v>81.441151880758568</v>
       </c>
-      <c r="I44" s="2">
-        <f>F44*H44</f>
-        <v>8.1441151880758564</v>
-      </c>
-      <c r="K44" s="2">
-        <f>I44-D44</f>
-        <v>0.14411518807585644</v>
-      </c>
-      <c r="L44" s="2">
-        <f t="shared" si="38"/>
-        <v>2.077E-2</v>
-      </c>
-      <c r="N44" s="2">
-        <f>2*F44*K44</f>
-        <v>2.8823037615171288E-2</v>
-      </c>
-      <c r="O44" s="2">
-        <f>E44*N44</f>
-        <v>0.51881467707308315</v>
-      </c>
-      <c r="P44" s="2">
-        <f t="shared" si="36"/>
-        <v>80.922337203685487</v>
-      </c>
-      <c r="R44" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U44" s="2">
-        <f t="shared" si="30"/>
-        <v>81.441151880758568</v>
-      </c>
       <c r="V44" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>2.077E-2</v>
       </c>
     </row>
     <row r="45" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>11</v>
       </c>
       <c r="D45" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F45" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="45"/>
+        <v>80.922337203685487</v>
+      </c>
+      <c r="I45" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E45" s="7">
+        <v>8.092233720368549</v>
+      </c>
+      <c r="K45" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F45" s="7">
-        <f>F44</f>
-        <v>0.1</v>
-      </c>
-      <c r="H45" s="2">
-        <f t="shared" si="35"/>
+        <v>9.2233720368549044E-2</v>
+      </c>
+      <c r="L45" s="2">
+        <f t="shared" si="48"/>
+        <v>8.5100000000000002E-3</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="36"/>
+        <v>1.844674407370981E-2</v>
+      </c>
+      <c r="O45" s="2">
+        <f t="shared" si="37"/>
+        <v>0.33204139332677657</v>
+      </c>
+      <c r="P45" s="2">
+        <f t="shared" si="46"/>
+        <v>80.590295810358711</v>
+      </c>
+      <c r="R45" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U45" s="2">
+        <f t="shared" si="39"/>
         <v>80.922337203685487</v>
       </c>
-      <c r="I45" s="2">
-        <f>F45*H45</f>
-        <v>8.092233720368549</v>
-      </c>
-      <c r="K45" s="2">
-        <f>I45-D45</f>
-        <v>9.2233720368549044E-2</v>
-      </c>
-      <c r="L45" s="2">
-        <f t="shared" si="38"/>
-        <v>8.5100000000000002E-3</v>
-      </c>
-      <c r="N45" s="2">
-        <f>2*F45*K45</f>
-        <v>1.844674407370981E-2</v>
-      </c>
-      <c r="O45" s="2">
-        <f>E45*N45</f>
-        <v>0.33204139332677657</v>
-      </c>
-      <c r="P45" s="2">
-        <f t="shared" si="36"/>
-        <v>80.590295810358711</v>
-      </c>
-      <c r="R45" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U45" s="2">
-        <f t="shared" si="30"/>
-        <v>80.922337203685487</v>
-      </c>
       <c r="V45" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>8.5100000000000002E-3</v>
       </c>
     </row>
     <row r="46" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>12</v>
       </c>
       <c r="D46" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E46" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F46" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="45"/>
+        <v>80.590295810358711</v>
+      </c>
+      <c r="I46" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E46" s="7">
+        <v>8.0590295810358707</v>
+      </c>
+      <c r="K46" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F46" s="7">
-        <f>F45</f>
-        <v>0.1</v>
-      </c>
-      <c r="H46" s="2">
-        <f t="shared" si="35"/>
+        <v>5.9029581035870748E-2</v>
+      </c>
+      <c r="L46" s="2">
+        <f t="shared" si="48"/>
+        <v>3.48E-3</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="36"/>
+        <v>1.1805916207174151E-2</v>
+      </c>
+      <c r="O46" s="2">
+        <f t="shared" si="37"/>
+        <v>0.21250649172913472</v>
+      </c>
+      <c r="P46" s="2">
+        <f t="shared" si="46"/>
+        <v>80.377789318629581</v>
+      </c>
+      <c r="R46" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U46" s="2">
+        <f t="shared" si="39"/>
         <v>80.590295810358711</v>
       </c>
-      <c r="I46" s="2">
-        <f>F46*H46</f>
-        <v>8.0590295810358707</v>
-      </c>
-      <c r="K46" s="2">
-        <f>I46-D46</f>
-        <v>5.9029581035870748E-2</v>
-      </c>
-      <c r="L46" s="2">
-        <f t="shared" si="38"/>
-        <v>3.48E-3</v>
-      </c>
-      <c r="N46" s="2">
-        <f>2*F46*K46</f>
-        <v>1.1805916207174151E-2</v>
-      </c>
-      <c r="O46" s="2">
-        <f>E46*N46</f>
-        <v>0.21250649172913472</v>
-      </c>
-      <c r="P46" s="2">
-        <f t="shared" si="36"/>
-        <v>80.377789318629581</v>
-      </c>
-      <c r="R46" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U46" s="2">
-        <f t="shared" si="30"/>
-        <v>80.590295810358711</v>
-      </c>
       <c r="V46" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>3.48E-3</v>
       </c>
     </row>
     <row r="47" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>13</v>
       </c>
       <c r="D47" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E47" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F47" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="45"/>
+        <v>80.377789318629581</v>
+      </c>
+      <c r="I47" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E47" s="7">
+        <v>8.0377789318629578</v>
+      </c>
+      <c r="K47" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F47" s="7">
-        <f>F46</f>
-        <v>0.1</v>
-      </c>
-      <c r="H47" s="2">
-        <f t="shared" si="35"/>
+        <v>3.7778931862957776E-2</v>
+      </c>
+      <c r="L47" s="2">
+        <f t="shared" si="48"/>
+        <v>1.4300000000000001E-3</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="36"/>
+        <v>7.5557863725915558E-3</v>
+      </c>
+      <c r="O47" s="2">
+        <f t="shared" si="37"/>
+        <v>0.13600415470664801</v>
+      </c>
+      <c r="P47" s="2">
+        <f t="shared" si="46"/>
+        <v>80.241785163922927</v>
+      </c>
+      <c r="R47" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U47" s="2">
+        <f t="shared" si="39"/>
         <v>80.377789318629581</v>
       </c>
-      <c r="I47" s="2">
-        <f>F47*H47</f>
-        <v>8.0377789318629578</v>
-      </c>
-      <c r="K47" s="2">
-        <f>I47-D47</f>
-        <v>3.7778931862957776E-2</v>
-      </c>
-      <c r="L47" s="2">
-        <f t="shared" si="38"/>
-        <v>1.4300000000000001E-3</v>
-      </c>
-      <c r="N47" s="2">
-        <f>2*F47*K47</f>
-        <v>7.5557863725915558E-3</v>
-      </c>
-      <c r="O47" s="2">
-        <f>E47*N47</f>
-        <v>0.13600415470664801</v>
-      </c>
-      <c r="P47" s="2">
-        <f t="shared" si="36"/>
-        <v>80.241785163922927</v>
-      </c>
-      <c r="R47" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U47" s="2">
-        <f t="shared" si="30"/>
-        <v>80.377789318629581</v>
-      </c>
       <c r="V47" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>1.4300000000000001E-3</v>
       </c>
     </row>
     <row r="48" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>14</v>
       </c>
       <c r="D48" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E48" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F48" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="45"/>
+        <v>80.241785163922927</v>
+      </c>
+      <c r="I48" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E48" s="7">
+        <v>8.0241785163922934</v>
+      </c>
+      <c r="K48" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F48" s="7">
-        <f>F47</f>
-        <v>0.1</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" si="35"/>
+        <v>2.4178516392293403E-2</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" si="48"/>
+        <v>5.8E-4</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="36"/>
+        <v>4.8357032784586808E-3</v>
+      </c>
+      <c r="O48" s="2">
+        <f t="shared" si="37"/>
+        <v>8.704265901225626E-2</v>
+      </c>
+      <c r="P48" s="2">
+        <f t="shared" si="46"/>
+        <v>80.154742504910672</v>
+      </c>
+      <c r="R48" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U48" s="2">
+        <f t="shared" si="39"/>
         <v>80.241785163922927</v>
       </c>
-      <c r="I48" s="2">
-        <f>F48*H48</f>
-        <v>8.0241785163922934</v>
-      </c>
-      <c r="K48" s="2">
-        <f>I48-D48</f>
-        <v>2.4178516392293403E-2</v>
-      </c>
-      <c r="L48" s="2">
-        <f t="shared" si="38"/>
-        <v>5.8E-4</v>
-      </c>
-      <c r="N48" s="2">
-        <f>2*F48*K48</f>
-        <v>4.8357032784586808E-3</v>
-      </c>
-      <c r="O48" s="2">
-        <f>E48*N48</f>
-        <v>8.704265901225626E-2</v>
-      </c>
-      <c r="P48" s="2">
-        <f t="shared" si="36"/>
-        <v>80.154742504910672</v>
-      </c>
-      <c r="R48" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U48" s="2">
-        <f t="shared" si="30"/>
-        <v>80.241785163922927</v>
-      </c>
       <c r="V48" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>5.8E-4</v>
       </c>
     </row>
     <row r="49" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>15</v>
       </c>
       <c r="D49" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E49" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F49" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="45"/>
+        <v>80.154742504910672</v>
+      </c>
+      <c r="I49" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E49" s="7">
+        <v>8.0154742504910672</v>
+      </c>
+      <c r="K49" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F49" s="7">
-        <f>F48</f>
-        <v>0.1</v>
-      </c>
-      <c r="H49" s="2">
-        <f t="shared" si="35"/>
+        <v>1.547425049106721E-2</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="48"/>
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="36"/>
+        <v>3.0948500982134423E-3</v>
+      </c>
+      <c r="O49" s="2">
+        <f t="shared" si="37"/>
+        <v>5.5707301767841957E-2</v>
+      </c>
+      <c r="P49" s="2">
+        <f t="shared" si="46"/>
+        <v>80.099035203142833</v>
+      </c>
+      <c r="R49" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U49" s="2">
+        <f t="shared" si="39"/>
         <v>80.154742504910672</v>
       </c>
-      <c r="I49" s="2">
-        <f>F49*H49</f>
-        <v>8.0154742504910672</v>
-      </c>
-      <c r="K49" s="2">
-        <f>I49-D49</f>
-        <v>1.547425049106721E-2</v>
-      </c>
-      <c r="L49" s="2">
-        <f t="shared" si="38"/>
-        <v>2.4000000000000001E-4</v>
-      </c>
-      <c r="N49" s="2">
-        <f>2*F49*K49</f>
-        <v>3.0948500982134423E-3</v>
-      </c>
-      <c r="O49" s="2">
-        <f>E49*N49</f>
-        <v>5.5707301767841957E-2</v>
-      </c>
-      <c r="P49" s="2">
-        <f t="shared" si="36"/>
-        <v>80.099035203142833</v>
-      </c>
-      <c r="R49" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U49" s="2">
-        <f t="shared" si="30"/>
-        <v>80.154742504910672</v>
-      </c>
       <c r="V49" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>2.4000000000000001E-4</v>
       </c>
     </row>
     <row r="50" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="41"/>
         <v>16</v>
       </c>
       <c r="D50" s="7">
+        <f t="shared" si="42"/>
+        <v>8</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="43"/>
+        <v>18</v>
+      </c>
+      <c r="F50" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="45"/>
+        <v>80.099035203142833</v>
+      </c>
+      <c r="I50" s="2">
         <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="E50" s="7">
+        <v>8.0099035203142837</v>
+      </c>
+      <c r="K50" s="2">
         <f t="shared" si="34"/>
-        <v>18</v>
-      </c>
-      <c r="F50" s="7">
-        <f>F49</f>
-        <v>0.1</v>
-      </c>
-      <c r="H50" s="2">
-        <f t="shared" si="35"/>
+        <v>9.9035203142836536E-3</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="48"/>
+        <v>1E-4</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="36"/>
+        <v>1.9807040628567309E-3</v>
+      </c>
+      <c r="O50" s="2">
+        <f t="shared" si="37"/>
+        <v>3.5652673131421155E-2</v>
+      </c>
+      <c r="P50" s="2">
+        <f t="shared" si="46"/>
+        <v>80.06338253001141</v>
+      </c>
+      <c r="R50" s="7" t="b">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="U50" s="2">
+        <f t="shared" si="39"/>
         <v>80.099035203142833</v>
       </c>
-      <c r="I50" s="2">
-        <f>F50*H50</f>
-        <v>8.0099035203142837</v>
-      </c>
-      <c r="K50" s="2">
-        <f>I50-D50</f>
-        <v>9.9035203142836536E-3</v>
-      </c>
-      <c r="L50" s="2">
-        <f t="shared" si="38"/>
-        <v>1E-4</v>
-      </c>
-      <c r="N50" s="2">
-        <f>2*F50*K50</f>
-        <v>1.9807040628567309E-3</v>
-      </c>
-      <c r="O50" s="2">
-        <f>E50*N50</f>
-        <v>3.5652673131421155E-2</v>
-      </c>
-      <c r="P50" s="2">
-        <f t="shared" si="36"/>
-        <v>80.06338253001141</v>
-      </c>
-      <c r="R50" s="7" t="b">
-        <f t="shared" si="29"/>
-        <v>1</v>
-      </c>
-      <c r="U50" s="2">
-        <f t="shared" si="30"/>
-        <v>80.099035203142833</v>
-      </c>
       <c r="V50" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="40"/>
         <v>1E-4</v>
       </c>
     </row>
     <row r="51" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="7">
-        <f t="shared" ref="B51:B54" si="39">B50+1</f>
+        <f t="shared" ref="B51:B54" si="49">B50+1</f>
         <v>17</v>
       </c>
       <c r="D51" s="7">
-        <f t="shared" ref="D51:D54" si="40">D50</f>
+        <f t="shared" ref="D51:D54" si="50">D50</f>
         <v>8</v>
       </c>
       <c r="E51" s="7">
-        <f t="shared" ref="E51:E54" si="41">E50</f>
+        <f t="shared" ref="E51:E54" si="51">E50</f>
         <v>18</v>
       </c>
       <c r="F51" s="7">
-        <f>F50</f>
+        <f t="shared" si="44"/>
         <v>0.1</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" ref="H51:H54" si="42">P50</f>
+        <f t="shared" ref="H51:H54" si="52">P50</f>
         <v>80.06338253001141</v>
       </c>
       <c r="I51" s="2">
-        <f>F51*H51</f>
+        <f t="shared" si="33"/>
         <v>8.0063382530011413</v>
       </c>
       <c r="K51" s="2">
-        <f>I51-D51</f>
+        <f t="shared" si="34"/>
         <v>6.3382530011413252E-3</v>
       </c>
       <c r="L51" s="2">
+        <f t="shared" si="48"/>
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="36"/>
+        <v>1.267650600228265E-3</v>
+      </c>
+      <c r="O51" s="2">
+        <f t="shared" si="37"/>
+        <v>2.2817710804108771E-2</v>
+      </c>
+      <c r="P51" s="2">
+        <f t="shared" ref="P51:P54" si="53">H51-O51</f>
+        <v>80.040564819207304</v>
+      </c>
+      <c r="R51" s="7" t="b">
         <f t="shared" si="38"/>
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="N51" s="2">
-        <f>2*F51*K51</f>
-        <v>1.267650600228265E-3</v>
-      </c>
-      <c r="O51" s="2">
-        <f>E51*N51</f>
-        <v>2.2817710804108771E-2</v>
-      </c>
-      <c r="P51" s="2">
-        <f t="shared" ref="P51:P54" si="43">H51-O51</f>
-        <v>80.040564819207304</v>
-      </c>
-      <c r="R51" s="7" t="b">
-        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="U51" s="2">
-        <f t="shared" ref="U51:U54" si="44">H51</f>
+        <f t="shared" ref="U51:U54" si="54">H51</f>
         <v>80.06338253001141</v>
       </c>
       <c r="V51" s="2">
-        <f t="shared" ref="V51:V54" si="45">L51</f>
+        <f t="shared" ref="V51:V54" si="55">L51</f>
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
     <row r="52" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="49"/>
         <v>18</v>
       </c>
       <c r="D52" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="50"/>
         <v>8</v>
       </c>
       <c r="E52" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="51"/>
         <v>18</v>
       </c>
       <c r="F52" s="7">
-        <f>F51</f>
+        <f t="shared" si="44"/>
         <v>0.1</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="52"/>
         <v>80.040564819207304</v>
       </c>
       <c r="I52" s="2">
-        <f>F52*H52</f>
+        <f t="shared" si="33"/>
         <v>8.0040564819207312</v>
       </c>
       <c r="K52" s="2">
-        <f>I52-D52</f>
+        <f t="shared" si="34"/>
         <v>4.0564819207311587E-3</v>
       </c>
       <c r="L52" s="2">
+        <f t="shared" si="48"/>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="36"/>
+        <v>8.1129638414623173E-4</v>
+      </c>
+      <c r="O52" s="2">
+        <f t="shared" si="37"/>
+        <v>1.4603334914632171E-2</v>
+      </c>
+      <c r="P52" s="2">
+        <f t="shared" si="53"/>
+        <v>80.025961484292679</v>
+      </c>
+      <c r="R52" s="7" t="b">
         <f t="shared" si="38"/>
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="N52" s="2">
-        <f>2*F52*K52</f>
-        <v>8.1129638414623173E-4</v>
-      </c>
-      <c r="O52" s="2">
-        <f>E52*N52</f>
-        <v>1.4603334914632171E-2</v>
-      </c>
-      <c r="P52" s="2">
-        <f t="shared" si="43"/>
-        <v>80.025961484292679</v>
-      </c>
-      <c r="R52" s="7" t="b">
-        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="U52" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="54"/>
         <v>80.040564819207304</v>
       </c>
       <c r="V52" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="55"/>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
     <row r="53" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="49"/>
         <v>19</v>
       </c>
       <c r="D53" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="50"/>
         <v>8</v>
       </c>
       <c r="E53" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="51"/>
         <v>18</v>
       </c>
       <c r="F53" s="7">
-        <f>F52</f>
+        <f t="shared" si="44"/>
         <v>0.1</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="52"/>
         <v>80.025961484292679</v>
       </c>
       <c r="I53" s="2">
-        <f>F53*H53</f>
+        <f t="shared" si="33"/>
         <v>8.0025961484292676</v>
       </c>
       <c r="K53" s="2">
-        <f>I53-D53</f>
+        <f t="shared" si="34"/>
         <v>2.5961484292675863E-3</v>
       </c>
       <c r="L53" s="2">
+        <f t="shared" si="48"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="36"/>
+        <v>5.1922968585351727E-4</v>
+      </c>
+      <c r="O53" s="2">
+        <f t="shared" si="37"/>
+        <v>9.3461343453633116E-3</v>
+      </c>
+      <c r="P53" s="2">
+        <f t="shared" si="53"/>
+        <v>80.016615349947315</v>
+      </c>
+      <c r="R53" s="7" t="b">
         <f t="shared" si="38"/>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="N53" s="2">
-        <f>2*F53*K53</f>
-        <v>5.1922968585351727E-4</v>
-      </c>
-      <c r="O53" s="2">
-        <f>E53*N53</f>
-        <v>9.3461343453633116E-3</v>
-      </c>
-      <c r="P53" s="2">
-        <f t="shared" si="43"/>
-        <v>80.016615349947315</v>
-      </c>
-      <c r="R53" s="7" t="b">
-        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="U53" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="54"/>
         <v>80.025961484292679</v>
       </c>
       <c r="V53" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="55"/>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="54" spans="2:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="7">
-        <f t="shared" si="39"/>
+        <f t="shared" si="49"/>
         <v>20</v>
       </c>
       <c r="D54" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="50"/>
         <v>8</v>
       </c>
       <c r="E54" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="51"/>
         <v>18</v>
       </c>
       <c r="F54" s="7">
-        <f>F53</f>
+        <f t="shared" si="44"/>
         <v>0.1</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="52"/>
         <v>80.016615349947315</v>
       </c>
       <c r="I54" s="2">
-        <f>F54*H54</f>
+        <f t="shared" si="33"/>
         <v>8.0016615349947315</v>
       </c>
       <c r="K54" s="2">
-        <f>I54-D54</f>
+        <f t="shared" si="34"/>
         <v>1.6615349947315394E-3</v>
       </c>
       <c r="L54" s="8">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="N54" s="2">
+        <f t="shared" si="36"/>
+        <v>3.3230699894630793E-4</v>
+      </c>
+      <c r="O54" s="2">
+        <f t="shared" si="37"/>
+        <v>5.9815259810335423E-3</v>
+      </c>
+      <c r="P54" s="2">
+        <f t="shared" si="53"/>
+        <v>80.010633823966288</v>
+      </c>
+      <c r="R54" s="17" t="b">
         <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="N54" s="2">
-        <f>2*F54*K54</f>
-        <v>3.3230699894630793E-4</v>
-      </c>
-      <c r="O54" s="2">
-        <f>E54*N54</f>
-        <v>5.9815259810335423E-3</v>
-      </c>
-      <c r="P54" s="2">
-        <f t="shared" si="43"/>
-        <v>80.010633823966288</v>
-      </c>
-      <c r="R54" s="27" t="b">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
       <c r="U54" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="54"/>
         <v>80.016615349947315</v>
       </c>
       <c r="V54" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="N32:P32"/>
+    <mergeCell ref="U32:V32"/>
+    <mergeCell ref="R32:R33"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="R6:R7"/>
     <mergeCell ref="V7:V8"/>
     <mergeCell ref="U6:V6"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="N32:P32"/>
-    <mergeCell ref="U32:V32"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="R32:R33"/>
-    <mergeCell ref="B32:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8107,7 +8103,7 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD7" sqref="AD7"/>
+      <selection pane="bottomLeft" activeCell="AD5" sqref="AD5:AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8134,15 +8130,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -8252,46 +8248,46 @@
       <c r="AB4" s="11"/>
     </row>
     <row r="5" spans="2:30" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="J5" s="18" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="J5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="O5" s="18" t="s">
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="O5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="18"/>
-      <c r="R5" s="18" t="s">
+      <c r="P5" s="23"/>
+      <c r="R5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AD5" s="26" t="s">
-        <v>111</v>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AD5" s="22" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:30" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="6"/>
       <c r="D6" s="13" t="s">
         <v>5</v>
@@ -8353,10 +8349,10 @@
       <c r="AB6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AD6" s="23"/>
+      <c r="AD6" s="20"/>
     </row>
     <row r="7" spans="2:30" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="6"/>
       <c r="D7" s="14" t="s">
         <v>31</v>
@@ -8424,7 +8420,7 @@
         <v>59</v>
       </c>
       <c r="AD7" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10483,20 +10479,20 @@
         <f t="shared" si="7"/>
         <v>4.9837466275460471E-2</v>
       </c>
-      <c r="AD30" s="27" t="b">
+      <c r="AD30" s="17" t="b">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="AD5:AD6"/>
     <mergeCell ref="D5:H5"/>
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="R5:AB5"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10512,7 +10508,7 @@
       <pane xSplit="2" ySplit="9" topLeftCell="Y123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AG127" sqref="AG127"/>
+      <selection pane="bottomRight" activeCell="AH137" sqref="AH137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10553,17 +10549,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
@@ -10608,116 +10604,116 @@
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="2:41" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
-      <c r="J6" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="T6" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AD6" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="18"/>
-      <c r="AH6" s="18"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="18"/>
-      <c r="AL6" s="18"/>
-      <c r="AN6" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="AO6" s="34"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+      <c r="J6" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="T6" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AD6" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="23"/>
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="23"/>
+      <c r="AL6" s="23"/>
+      <c r="AN6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO6" s="28"/>
     </row>
     <row r="7" spans="2:41" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
-      <c r="J7" s="17" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="J7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="17"/>
-      <c r="M7" s="17" t="s">
+      <c r="K7" s="21"/>
+      <c r="M7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="17"/>
-      <c r="P7" s="17" t="s">
+      <c r="N7" s="21"/>
+      <c r="P7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="T7" s="17" t="s">
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="T7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="U7" s="17"/>
-      <c r="W7" s="17" t="s">
+      <c r="U7" s="21"/>
+      <c r="W7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="X7" s="17"/>
-      <c r="Z7" s="17" t="s">
+      <c r="X7" s="21"/>
+      <c r="Z7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
-      <c r="AD7" s="17" t="s">
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AD7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AE7" s="17"/>
-      <c r="AG7" s="17" t="s">
+      <c r="AE7" s="21"/>
+      <c r="AG7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="AH7" s="17"/>
-      <c r="AJ7" s="17" t="s">
+      <c r="AH7" s="21"/>
+      <c r="AJ7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AK7" s="17"/>
-      <c r="AL7" s="17"/>
-      <c r="AN7" s="34"/>
-      <c r="AO7" s="34"/>
+      <c r="AK7" s="21"/>
+      <c r="AL7" s="21"/>
+      <c r="AN7" s="28"/>
+      <c r="AO7" s="28"/>
     </row>
     <row r="8" spans="2:41" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="6"/>
       <c r="D8" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>4</v>
@@ -10729,83 +10725,83 @@
         <v>19</v>
       </c>
       <c r="K8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="N8" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="N8" s="13" t="s">
+      <c r="P8" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="P8" s="13" t="s">
+      <c r="Q8" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="Q8" s="13" t="s">
+      <c r="R8" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="R8" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="T8" s="13" t="s">
         <v>20</v>
       </c>
       <c r="U8" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="W8" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="X8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="W8" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="X8" s="13" t="s">
+      <c r="Z8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="Z8" s="13" t="s">
+      <c r="AA8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="AA8" s="13" t="s">
+      <c r="AB8" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="AB8" s="13" t="s">
-        <v>88</v>
       </c>
       <c r="AD8" s="13" t="s">
         <v>21</v>
       </c>
       <c r="AE8" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH8" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="AH8" s="13" t="s">
+      <c r="AJ8" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="AJ8" s="13" t="s">
+      <c r="AK8" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="AK8" s="13" t="s">
+      <c r="AL8" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="AL8" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN8" s="24" t="s">
+      <c r="AN8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AO8" s="16" t="s">
         <v>110</v>
-      </c>
-      <c r="AO8" s="24" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" spans="2:41" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="6"/>
       <c r="D9" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>29</v>
@@ -10818,21 +10814,21 @@
         <v>41</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>79</v>
       </c>
       <c r="O9" s="15"/>
       <c r="P9" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R9" s="14" t="s">
         <v>61</v>
@@ -10841,53 +10837,53 @@
         <v>42</v>
       </c>
       <c r="U9" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V9" s="15"/>
       <c r="W9" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="X9" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="X9" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="Y9" s="15"/>
       <c r="Z9" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA9" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB9" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="AB9" s="14" t="s">
-        <v>93</v>
-      </c>
       <c r="AD9" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE9" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="AE9" s="14" t="s">
-        <v>104</v>
       </c>
       <c r="AF9" s="15"/>
       <c r="AG9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH9" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="AH9" s="14" t="s">
-        <v>106</v>
       </c>
       <c r="AI9" s="15"/>
       <c r="AJ9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AK9" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="AK9" s="14" t="s">
+      <c r="AL9" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="AL9" s="14" t="s">
-        <v>109</v>
-      </c>
       <c r="AN9" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AO9" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -25043,11 +25039,10 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AD6:AL6"/>
-    <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="AN6:AO7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:H7"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="P7:R7"/>
     <mergeCell ref="J6:R6"/>
@@ -25055,10 +25050,11 @@
     <mergeCell ref="T7:U7"/>
     <mergeCell ref="W7:X7"/>
     <mergeCell ref="Z7:AB7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:H7"/>
-    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="AD6:AL6"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AG7:AH7"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="AN6:AO7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>